<commit_message>
Price list 2.0 20.03.18
</commit_message>
<xml_diff>
--- a/assets/price/price_src.xlsx
+++ b/assets/price/price_src.xlsx
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +714,7 @@
         <v>30</v>
       </c>
       <c r="C13">
-        <v>543</v>
+        <v>582</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>